<commit_message>
Next commit to GitHub.
</commit_message>
<xml_diff>
--- a/data_result_with_the_summ.xlsx
+++ b/data_result_with_the_summ.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="256">
   <si>
     <t xml:space="preserve">1:</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve"> 1958₽</t>
   </si>
   <si>
-    <t xml:space="preserve">https://basket-10.wb.ru/vol1377/part137790/137790056/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/137790056/detail.aspx?size=234503434</t>
   </si>
   <si>
     <t xml:space="preserve">2:</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> 585₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-09.wb.ru/vol1229/part122932/122932874/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/122932874/detail.aspx?size=216462701</t>
   </si>
   <si>
     <t xml:space="preserve">3:</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve"> 394₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol511/part51131/51131942/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/51131942/detail.aspx?size=96806803</t>
   </si>
   <si>
     <t xml:space="preserve">4:</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve"> 251₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-02.wb.ru/vol199/part19924/19924600/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/19924600/detail.aspx?size=52491178</t>
   </si>
   <si>
     <t xml:space="preserve">5:</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve"> 297₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol812/part81296/81296702/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/81296702/detail.aspx?size=134329081</t>
   </si>
   <si>
     <t xml:space="preserve">6:</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve"> 85₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol382/part38211/38211868/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/38211868/detail.aspx?size=78253310</t>
   </si>
   <si>
     <t xml:space="preserve">7:</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve"> 902₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-01.wb.ru/vol130/part13015/13015303/images/c516x688/1.webp</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/13015303/detail.aspx?size=39867586</t>
   </si>
   <si>
     <t xml:space="preserve">8:</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve"> 248₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol514/part51422/51422945/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/51422945/detail.aspx?size=97168418</t>
   </si>
   <si>
     <t xml:space="preserve">9:</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve"> 749₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol912/part91290/91290847/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/91290847/detail.aspx?size=146841365</t>
   </si>
   <si>
     <t xml:space="preserve">11:</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve"> 269₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1339/part133908/133908820/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/133908820/detail.aspx?size=229749167</t>
   </si>
   <si>
     <t xml:space="preserve">13:</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve"> 172₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol359/part35924/35924822/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/35924822/detail.aspx?size=75016837</t>
   </si>
   <si>
     <t xml:space="preserve">17:</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve"> 79₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-07.wb.ru/vol1065/part106588/106588004/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/106588004/detail.aspx?size=166618905</t>
   </si>
   <si>
     <t xml:space="preserve">18:</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve"> 5124₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol988/part98836/98836160/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/98836160/detail.aspx?size=156186676</t>
   </si>
   <si>
     <t xml:space="preserve">19:</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve"> 1051₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol409/part40997/40997355/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/40997355/detail.aspx?size=82618219</t>
   </si>
   <si>
     <t xml:space="preserve">20:</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve"> 772₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1342/part134283/134283474/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/134283474/detail.aspx?size=230255831</t>
   </si>
   <si>
     <t xml:space="preserve">21:</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve"> Dorez / Дождевик пончо</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1394/part139466/139466508/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/139466508/detail.aspx?size=236745366</t>
   </si>
   <si>
     <t xml:space="preserve">22:</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve"> АЛЬФАПЛАСТИК / Жгут кровоостанавливающий резиновый Эсмарха</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1381/part138108/138108792/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/138108792/detail.aspx?size=234955112</t>
   </si>
   <si>
     <t xml:space="preserve">23:</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve"> 1216₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol297/part29720/29720306/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/29720306/detail.aspx?size=66115928</t>
   </si>
   <si>
     <t xml:space="preserve">24:</t>
@@ -256,7 +256,7 @@
     <t xml:space="preserve"> 299₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol484/part48439/48439526/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/48439526/detail.aspx?size=93238774</t>
   </si>
   <si>
     <t xml:space="preserve">25:</t>
@@ -268,7 +268,7 @@
     <t xml:space="preserve"> 823₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1356/part135632/135632152/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/135632152/detail.aspx?size=231859869</t>
   </si>
   <si>
     <t xml:space="preserve">26:</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve"> 972₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1408/part140830/140830250/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/140830250/detail.aspx?size=238677619</t>
   </si>
   <si>
     <t xml:space="preserve">27:</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve"> 493₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol910/part91023/91023003/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/91023003/detail.aspx?size=146459226</t>
   </si>
   <si>
     <t xml:space="preserve">28:</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve"> 1464₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-02.wb.ru/vol258/part25817/25817631/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/25817631/detail.aspx?size=59950948</t>
   </si>
   <si>
     <t xml:space="preserve">29:</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve"> 88₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-08.wb.ru/vol1116/part111648/111648768/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/111648768/detail.aspx?size=202098968</t>
   </si>
   <si>
     <t xml:space="preserve">30:</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve"> 737₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-07.wb.ru/vol1073/part107341/107341531/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/107341531/detail.aspx?size=167432318</t>
   </si>
   <si>
     <t xml:space="preserve">31:</t>
@@ -340,7 +340,7 @@
     <t xml:space="preserve"> 252₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-09.wb.ru/vol1279/part127950/127950425/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/127950425/detail.aspx?size=222865939</t>
   </si>
   <si>
     <t xml:space="preserve">32:</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve"> НИТЕКС / Сети маскировочные</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol345/part34529/34529600/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/34529600/detail.aspx?size=72636500</t>
   </si>
   <si>
     <t xml:space="preserve">34:</t>
@@ -364,7 +364,7 @@
     <t xml:space="preserve"> 544₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol975/part97577/97577053/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/97577053/detail.aspx?size=154644828</t>
   </si>
   <si>
     <t xml:space="preserve">35:</t>
@@ -376,7 +376,7 @@
     <t xml:space="preserve"> 239₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol954/part95488/95488793/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/95488793/detail.aspx?size=152057910</t>
   </si>
   <si>
     <t xml:space="preserve">36:</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve"> 1196₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-07.wb.ru/vol1062/part106263/106263958/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/106263958/detail.aspx?size=166194736</t>
   </si>
   <si>
     <t xml:space="preserve">37:</t>
@@ -403,7 +403,7 @@
     <t xml:space="preserve"> 665₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1390/part139086/139086756/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/139086756/detail.aspx?size=236213883</t>
   </si>
   <si>
     <t xml:space="preserve">39:</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve"> 437₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-08.wb.ru/vol1147/part114704/114704390/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/114704390/detail.aspx?size=205924493</t>
   </si>
   <si>
     <t xml:space="preserve">40:</t>
@@ -427,7 +427,7 @@
     <t xml:space="preserve"> 728₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1388/part138878/138878415/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/138878415/detail.aspx?size=235917000</t>
   </si>
   <si>
     <t xml:space="preserve">41:</t>
@@ -439,7 +439,7 @@
     <t xml:space="preserve"> 283₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol294/part29441/29441802/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/29441802/detail.aspx?size=65719769</t>
   </si>
   <si>
     <t xml:space="preserve">42:</t>
@@ -451,7 +451,7 @@
     <t xml:space="preserve"> 1267₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol346/part34613/34613666/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/34613666/detail.aspx?size=72752256</t>
   </si>
   <si>
     <t xml:space="preserve">43:</t>
@@ -463,7 +463,7 @@
     <t xml:space="preserve"> 335₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol783/part78356/78356949/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/78356949/detail.aspx?size=130812247</t>
   </si>
   <si>
     <t xml:space="preserve">44:</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve"> 1395₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol611/part61142/61142587/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/61142587/detail.aspx?size=108608117</t>
   </si>
   <si>
     <t xml:space="preserve">45:</t>
@@ -487,7 +487,7 @@
     <t xml:space="preserve"> 133₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-08.wb.ru/vol1116/part111648/111648767/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/111648767/detail.aspx?size=202098967</t>
   </si>
   <si>
     <t xml:space="preserve">46:</t>
@@ -499,13 +499,7 @@
     <t xml:space="preserve"> 135₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1397/part139714/139714376/images/c516x688/1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.wildberries.ru/catalog/137790056/detail.aspx?size=234503434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.wildberries.ru/catalog/122932874/detail.aspx?size=216462701</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/139714376/detail.aspx?size=237044569</t>
   </si>
   <si>
     <t xml:space="preserve">47:</t>
@@ -517,10 +511,7 @@
     <t xml:space="preserve"> 542₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol949/part94931/94931522/images/c516x688/1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/94931522/detail.aspx?size=151354545</t>
   </si>
   <si>
     <t xml:space="preserve">48:</t>
@@ -532,7 +523,7 @@
     <t xml:space="preserve"> 714₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1355/part135544/135544299/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/135544299/detail.aspx?size=231746676</t>
   </si>
   <si>
     <t xml:space="preserve">49:</t>
@@ -544,7 +535,7 @@
     <t xml:space="preserve"> 352₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1356/part135661/135661717/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/135661717/detail.aspx?size=231895417</t>
   </si>
   <si>
     <t xml:space="preserve">50:</t>
@@ -556,7 +547,7 @@
     <t xml:space="preserve"> 194₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol397/part39724/39724468/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/39724468/detail.aspx?size=80384369</t>
   </si>
   <si>
     <t xml:space="preserve">51:</t>
@@ -568,7 +559,7 @@
     <t xml:space="preserve"> 216₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol637/part63774/63774014/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/63774014/detail.aspx?size=112052920</t>
   </si>
   <si>
     <t xml:space="preserve">52:</t>
@@ -580,7 +571,7 @@
     <t xml:space="preserve"> 316₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1378/part137887/137887117/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/137887117/detail.aspx?size=234648174</t>
   </si>
   <si>
     <t xml:space="preserve">53:</t>
@@ -592,7 +583,7 @@
     <t xml:space="preserve"> 366₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol625/part62558/62558967/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/62558967/detail.aspx?size=110492146</t>
   </si>
   <si>
     <t xml:space="preserve">54:</t>
@@ -604,7 +595,7 @@
     <t xml:space="preserve"> 249₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-02.wb.ru/vol152/part15234/15234660/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/15234660/detail.aspx?size=44448766</t>
   </si>
   <si>
     <t xml:space="preserve">55:</t>
@@ -616,7 +607,7 @@
     <t xml:space="preserve"> 141₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol443/part44347/44347490/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/44347490/detail.aspx?size=87699855</t>
   </si>
   <si>
     <t xml:space="preserve">56:</t>
@@ -628,7 +619,7 @@
     <t xml:space="preserve"> 816₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1408/part140845/140845029/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/140845029/detail.aspx?size=238697536</t>
   </si>
   <si>
     <t xml:space="preserve">57:</t>
@@ -640,7 +631,7 @@
     <t xml:space="preserve"> 253₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-05.wb.ru/vol994/part99478/99478471/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/99478471/detail.aspx?size=156975726</t>
   </si>
   <si>
     <t xml:space="preserve">58:</t>
@@ -652,7 +643,7 @@
     <t xml:space="preserve"> 266₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-10.wb.ru/vol1374/part137455/137455591/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/137455591/detail.aspx?size=234026464</t>
   </si>
   <si>
     <t xml:space="preserve">59:</t>
@@ -664,7 +655,7 @@
     <t xml:space="preserve"> 686₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol418/part41807/41807306/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/41807306/detail.aspx?size=83873345</t>
   </si>
   <si>
     <t xml:space="preserve">60:</t>
@@ -676,7 +667,7 @@
     <t xml:space="preserve"> 108₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol496/part49601/49601048/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/49601048/detail.aspx?size=94824237</t>
   </si>
   <si>
     <t xml:space="preserve">61:</t>
@@ -688,7 +679,7 @@
     <t xml:space="preserve"> 590₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-04.wb.ru/vol501/part50108/50108997/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/50108997/detail.aspx?size=95533060</t>
   </si>
   <si>
     <t xml:space="preserve">62:</t>
@@ -700,7 +691,7 @@
     <t xml:space="preserve"> 280₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-02.wb.ru/vol164/part16441/16441221/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/16441221/detail.aspx?size=46691487</t>
   </si>
   <si>
     <t xml:space="preserve">63:</t>
@@ -712,7 +703,7 @@
     <t xml:space="preserve"> 225₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-06.wb.ru/vol1052/part105227/105227835/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/105227835/detail.aspx?size=164825123</t>
   </si>
   <si>
     <t xml:space="preserve">64:</t>
@@ -724,19 +715,90 @@
     <t xml:space="preserve"> 608₽</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://basket-03.wb.ru/vol425/part42521/42521372/images/c516x688/1.jpg</t>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/42521372/detail.aspx?size=85027912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Карабинер / Браслет тактический из паракорда</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 292₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/90644597/detail.aspx?size=145957016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hobbyxit / Армейская фляга (фляжка) с алюминиевым котелком рыбалка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1465₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/29336607/detail.aspx?size=65562586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOURGAN / Термоодеяло спасательное туристическое военное 160х210</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 576₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/122424599/detail.aspx?size=215565875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Оранжевое яблоко / Фонарик налобный аккумуляторный</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 320₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/66175703/detail.aspx?size=115125187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Image / Сухое горючее</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 117₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/26457344/detail.aspx?size=61091120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CANYON / Внешний аккумулятор с функцией быстрой зарядки PB-107, 10000…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 506₽</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.wildberries.ru/catalog/117913774/detail.aspx?size=209949633</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$RUB];\-#,##0.00\ [$RUB]"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -756,12 +818,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -806,25 +862,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -844,30 +888,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I93" activeCellId="0" sqref="I93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D103" activeCellId="0" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="83.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="63.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -875,11 +917,6 @@
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="1" t="n">
-        <f aca="false">E1*F1</f>
-        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,23 +926,19 @@
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="0" t="n">
         <f aca="false">A2</f>
         <v>1958</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">E2*F2</f>
-        <v>1958</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -913,11 +946,6 @@
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="n">
-        <f aca="false">E3*F3</f>
-        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,23 +955,19 @@
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="0" t="n">
         <f aca="false">A4</f>
         <v>585</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <f aca="false">E4*F4</f>
-        <v>585</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -951,11 +975,6 @@
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1" t="n">
-        <f aca="false">E5*F5</f>
-        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,23 +984,19 @@
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="0" t="n">
         <f aca="false">A6</f>
         <v>394</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <f aca="false">E6*F6</f>
-        <v>394</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -989,11 +1004,6 @@
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1" t="n">
-        <f aca="false">E7*F7</f>
-        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,23 +1013,19 @@
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="0" t="n">
         <f aca="false">A8</f>
         <v>251</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <f aca="false">E8*F8</f>
-        <v>251</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1027,11 +1033,6 @@
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="1" t="n">
-        <f aca="false">E9*F9</f>
-        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,23 +1042,19 @@
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="0" t="n">
         <f aca="false">A10</f>
         <v>297</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <f aca="false">E10*F10</f>
-        <v>297</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -1065,11 +1062,6 @@
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="1" t="n">
-        <f aca="false">E11*F11</f>
-        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,23 +1071,19 @@
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="0" t="n">
         <f aca="false">A12</f>
         <v>85</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <f aca="false">E12*F12</f>
-        <v>85</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -1103,11 +1091,6 @@
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1" t="n">
-        <f aca="false">E13*F13</f>
-        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,23 +1100,19 @@
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="0" t="n">
         <f aca="false">A14</f>
         <v>902</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <f aca="false">E14*F14</f>
-        <v>902</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -1141,11 +1120,6 @@
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1" t="n">
-        <f aca="false">E15*F15</f>
-        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,23 +1129,19 @@
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="0" t="n">
         <f aca="false">A16</f>
         <v>248</v>
       </c>
-      <c r="G16" s="1" t="n">
-        <f aca="false">E16*F16</f>
-        <v>248</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -1179,11 +1149,6 @@
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="1" t="n">
-        <f aca="false">E17*F17</f>
-        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,23 +1158,19 @@
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="0" t="n">
         <f aca="false">A18</f>
         <v>85</v>
       </c>
-      <c r="G18" s="1" t="n">
-        <f aca="false">E18*F18</f>
-        <v>85</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="0" t="s">
@@ -1217,11 +1178,6 @@
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="1" t="n">
-        <f aca="false">E19*F19</f>
-        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,23 +1187,19 @@
       <c r="E20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="0" t="n">
         <f aca="false">A20</f>
         <v>749</v>
       </c>
-      <c r="G20" s="1" t="n">
-        <f aca="false">E20*F20</f>
-        <v>749</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="0" t="s">
@@ -1255,11 +1207,6 @@
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="1" t="n">
-        <f aca="false">E21*F21</f>
-        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,23 +1216,19 @@
       <c r="E22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="0" t="n">
         <f aca="false">A22</f>
         <v>248</v>
       </c>
-      <c r="G22" s="1" t="n">
-        <f aca="false">E22*F22</f>
-        <v>248</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="0" t="s">
@@ -1293,11 +1236,6 @@
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="1" t="n">
-        <f aca="false">E23*F23</f>
-        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,23 +1245,19 @@
       <c r="E24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="0" t="n">
         <f aca="false">A24</f>
         <v>269</v>
       </c>
-      <c r="G24" s="1" t="n">
-        <f aca="false">E24*F24</f>
-        <v>269</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="0" t="s">
@@ -1331,11 +1265,6 @@
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="1" t="n">
-        <f aca="false">E25*F25</f>
-        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,23 +1274,19 @@
       <c r="E26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="0" t="n">
         <f aca="false">A26</f>
         <v>251</v>
       </c>
-      <c r="G26" s="1" t="n">
-        <f aca="false">E26*F26</f>
-        <v>251</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="0" t="s">
@@ -1369,11 +1294,6 @@
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="1" t="n">
-        <f aca="false">E27*F27</f>
-        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,23 +1303,19 @@
       <c r="E28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="0" t="n">
         <f aca="false">A28</f>
         <v>749</v>
       </c>
-      <c r="G28" s="1" t="n">
-        <f aca="false">E28*F28</f>
-        <v>749</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="0" t="s">
@@ -1407,11 +1323,6 @@
       </c>
       <c r="E29" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="1" t="n">
-        <f aca="false">E29*F29</f>
-        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,23 +1332,19 @@
       <c r="E30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="0" t="n">
         <f aca="false">A30</f>
         <v>269</v>
       </c>
-      <c r="G30" s="1" t="n">
-        <f aca="false">E30*F30</f>
-        <v>269</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="0" t="s">
@@ -1445,11 +1352,6 @@
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="1" t="n">
-        <f aca="false">E31*F31</f>
-        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,23 +1361,19 @@
       <c r="E32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="0" t="n">
         <f aca="false">A32</f>
         <v>172</v>
       </c>
-      <c r="G32" s="1" t="n">
-        <f aca="false">E32*F32</f>
-        <v>172</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="0" t="s">
@@ -1483,11 +1381,6 @@
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="1" t="n">
-        <f aca="false">E33*F33</f>
-        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,23 +1390,19 @@
       <c r="E34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="0" t="n">
         <f aca="false">A34</f>
         <v>79</v>
       </c>
-      <c r="G34" s="1" t="n">
-        <f aca="false">E34*F34</f>
-        <v>79</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="0" t="s">
@@ -1521,11 +1410,6 @@
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="1" t="n">
-        <f aca="false">E35*F35</f>
-        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,23 +1419,19 @@
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="0" t="n">
         <f aca="false">A36</f>
         <v>5124</v>
       </c>
-      <c r="G36" s="1" t="n">
-        <f aca="false">E36*F36</f>
-        <v>5124</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D37" s="0" t="s">
@@ -1559,11 +1439,6 @@
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="1" t="n">
-        <f aca="false">E37*F37</f>
-        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,23 +1448,19 @@
       <c r="E38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="0" t="n">
         <f aca="false">A38</f>
         <v>1051</v>
       </c>
-      <c r="G38" s="1" t="n">
-        <f aca="false">E38*F38</f>
-        <v>1051</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -1597,11 +1468,6 @@
       </c>
       <c r="E39" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="1" t="n">
-        <f aca="false">E39*F39</f>
-        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,23 +1477,19 @@
       <c r="E40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="0" t="n">
         <f aca="false">A40</f>
         <v>772</v>
       </c>
-      <c r="G40" s="1" t="n">
-        <f aca="false">E40*F40</f>
-        <v>772</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D41" s="0" t="s">
@@ -1635,11 +1497,6 @@
       </c>
       <c r="E41" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="1" t="n">
-        <f aca="false">E41*F41</f>
-        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,23 +1506,19 @@
       <c r="E42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="0" t="n">
         <f aca="false">A42</f>
         <v>772</v>
       </c>
-      <c r="G42" s="1" t="n">
-        <f aca="false">E42*F42</f>
-        <v>772</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="0" t="s">
@@ -1673,11 +1526,6 @@
       </c>
       <c r="E43" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="1" t="n">
-        <f aca="false">E43*F43</f>
-        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,23 +1535,19 @@
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="0" t="n">
         <f aca="false">A44</f>
         <v>269</v>
       </c>
-      <c r="G44" s="1" t="n">
-        <f aca="false">E44*F44</f>
-        <v>269</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D45" s="0" t="s">
@@ -1711,11 +1555,6 @@
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="1" t="n">
-        <f aca="false">E45*F45</f>
-        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,23 +1564,19 @@
       <c r="E46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="0" t="n">
         <f aca="false">A46</f>
         <v>1216</v>
       </c>
-      <c r="G46" s="1" t="n">
-        <f aca="false">E46*F46</f>
-        <v>1216</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D47" s="0" t="s">
@@ -1749,11 +1584,6 @@
       </c>
       <c r="E47" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="1" t="n">
-        <f aca="false">E47*F47</f>
-        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,23 +1593,19 @@
       <c r="E48" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F48" s="4" t="n">
+      <c r="F48" s="0" t="n">
         <f aca="false">A48</f>
         <v>299</v>
       </c>
-      <c r="G48" s="1" t="n">
-        <f aca="false">E48*F48</f>
-        <v>299</v>
-      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D49" s="0" t="s">
@@ -1787,11 +1613,6 @@
       </c>
       <c r="E49" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="1" t="n">
-        <f aca="false">E49*F49</f>
-        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,23 +1622,19 @@
       <c r="E50" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="0" t="n">
         <f aca="false">A50</f>
         <v>823</v>
       </c>
-      <c r="G50" s="1" t="n">
-        <f aca="false">E50*F50</f>
-        <v>823</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D51" s="0" t="s">
@@ -1825,11 +1642,6 @@
       </c>
       <c r="E51" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="1" t="n">
-        <f aca="false">E51*F51</f>
-        <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,23 +1651,19 @@
       <c r="E52" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="0" t="n">
         <f aca="false">A52</f>
         <v>972</v>
       </c>
-      <c r="G52" s="1" t="n">
-        <f aca="false">E52*F52</f>
-        <v>972</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D53" s="0" t="s">
@@ -1863,11 +1671,6 @@
       </c>
       <c r="E53" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="1" t="n">
-        <f aca="false">E53*F53</f>
-        <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,23 +1680,19 @@
       <c r="E54" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F54" s="4" t="n">
+      <c r="F54" s="0" t="n">
         <f aca="false">A54</f>
         <v>493</v>
       </c>
-      <c r="G54" s="1" t="n">
-        <f aca="false">E54*F54</f>
-        <v>493</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D55" s="0" t="s">
@@ -1901,11 +1700,6 @@
       </c>
       <c r="E55" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="1" t="n">
-        <f aca="false">E55*F55</f>
-        <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,23 +1709,19 @@
       <c r="E56" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F56" s="4" t="n">
+      <c r="F56" s="0" t="n">
         <f aca="false">A56</f>
         <v>1464</v>
       </c>
-      <c r="G56" s="1" t="n">
-        <f aca="false">E56*F56</f>
-        <v>1464</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D57" s="0" t="s">
@@ -1939,11 +1729,6 @@
       </c>
       <c r="E57" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="1" t="n">
-        <f aca="false">E57*F57</f>
-        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,23 +1738,19 @@
       <c r="E58" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="0" t="n">
         <f aca="false">A58</f>
         <v>88</v>
       </c>
-      <c r="G58" s="1" t="n">
-        <f aca="false">E58*F58</f>
-        <v>88</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D59" s="0" t="s">
@@ -1977,11 +1758,6 @@
       </c>
       <c r="E59" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="1" t="n">
-        <f aca="false">E59*F59</f>
-        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,23 +1767,19 @@
       <c r="E60" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F60" s="4" t="n">
+      <c r="F60" s="0" t="n">
         <f aca="false">A60</f>
         <v>737</v>
       </c>
-      <c r="G60" s="1" t="n">
-        <f aca="false">E60*F60</f>
-        <v>737</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D61" s="0" t="s">
@@ -2015,11 +1787,6 @@
       </c>
       <c r="E61" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="1" t="n">
-        <f aca="false">E61*F61</f>
-        <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,23 +1796,19 @@
       <c r="E62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F62" s="4" t="n">
+      <c r="F62" s="0" t="n">
         <f aca="false">A62</f>
         <v>252</v>
       </c>
-      <c r="G62" s="1" t="n">
-        <f aca="false">E62*F62</f>
-        <v>252</v>
-      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D63" s="0" t="s">
@@ -2053,11 +1816,6 @@
       </c>
       <c r="E63" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="1" t="n">
-        <f aca="false">E63*F63</f>
-        <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,23 +1825,19 @@
       <c r="E64" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F64" s="4" t="n">
+      <c r="F64" s="0" t="n">
         <f aca="false">A64</f>
         <v>772</v>
       </c>
-      <c r="G64" s="1" t="n">
-        <f aca="false">E64*F64</f>
-        <v>772</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D65" s="0" t="s">
@@ -2091,11 +1845,6 @@
       </c>
       <c r="E65" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="1" t="n">
-        <f aca="false">E65*F65</f>
-        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,23 +1854,19 @@
       <c r="E66" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F66" s="4" t="n">
+      <c r="F66" s="0" t="n">
         <f aca="false">A66</f>
         <v>902</v>
       </c>
-      <c r="G66" s="1" t="n">
-        <f aca="false">E66*F66</f>
-        <v>902</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D67" s="0" t="s">
@@ -2129,11 +1874,6 @@
       </c>
       <c r="E67" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F67" s="4"/>
-      <c r="G67" s="1" t="n">
-        <f aca="false">E67*F67</f>
-        <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,23 +1883,19 @@
       <c r="E68" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F68" s="4" t="n">
+      <c r="F68" s="0" t="n">
         <f aca="false">A68</f>
         <v>544</v>
       </c>
-      <c r="G68" s="1" t="n">
-        <f aca="false">E68*F68</f>
-        <v>544</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D69" s="0" t="s">
@@ -2167,11 +1903,6 @@
       </c>
       <c r="E69" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F69" s="4"/>
-      <c r="G69" s="1" t="n">
-        <f aca="false">E69*F69</f>
-        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,23 +1912,19 @@
       <c r="E70" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F70" s="4" t="n">
+      <c r="F70" s="0" t="n">
         <f aca="false">A70</f>
         <v>239</v>
       </c>
-      <c r="G70" s="1" t="n">
-        <f aca="false">E70*F70</f>
-        <v>239</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D71" s="0" t="s">
@@ -2205,11 +1932,6 @@
       </c>
       <c r="E71" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="1" t="n">
-        <f aca="false">E71*F71</f>
-        <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,23 +1941,19 @@
       <c r="E72" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F72" s="4" t="n">
+      <c r="F72" s="0" t="n">
         <f aca="false">A72</f>
         <v>1196</v>
       </c>
-      <c r="G72" s="1" t="n">
-        <f aca="false">E72*F72</f>
-        <v>1196</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D73" s="0" t="s">
@@ -2243,11 +1961,6 @@
       </c>
       <c r="E73" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F73" s="4"/>
-      <c r="G73" s="1" t="n">
-        <f aca="false">E73*F73</f>
-        <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,23 +1970,19 @@
       <c r="E74" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F74" s="4" t="n">
+      <c r="F74" s="0" t="n">
         <f aca="false">A74</f>
         <v>239</v>
       </c>
-      <c r="G74" s="1" t="n">
-        <f aca="false">E74*F74</f>
-        <v>239</v>
-      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D75" s="0" t="s">
@@ -2281,11 +1990,6 @@
       </c>
       <c r="E75" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F75" s="4"/>
-      <c r="G75" s="1" t="n">
-        <f aca="false">E75*F75</f>
-        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,23 +1999,19 @@
       <c r="E76" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F76" s="4" t="n">
+      <c r="F76" s="0" t="n">
         <f aca="false">A76</f>
         <v>665</v>
       </c>
-      <c r="G76" s="1" t="n">
-        <f aca="false">E76*F76</f>
-        <v>665</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D77" s="0" t="s">
@@ -2319,11 +2019,6 @@
       </c>
       <c r="E77" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F77" s="4"/>
-      <c r="G77" s="1" t="n">
-        <f aca="false">E77*F77</f>
-        <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,23 +2028,19 @@
       <c r="E78" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F78" s="4" t="n">
+      <c r="F78" s="0" t="n">
         <f aca="false">A78</f>
         <v>437</v>
       </c>
-      <c r="G78" s="1" t="n">
-        <f aca="false">E78*F78</f>
-        <v>437</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D79" s="0" t="s">
@@ -2357,11 +2048,6 @@
       </c>
       <c r="E79" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F79" s="4"/>
-      <c r="G79" s="1" t="n">
-        <f aca="false">E79*F79</f>
-        <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,23 +2057,19 @@
       <c r="E80" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F80" s="4" t="n">
+      <c r="F80" s="0" t="n">
         <f aca="false">A80</f>
         <v>728</v>
       </c>
-      <c r="G80" s="1" t="n">
-        <f aca="false">E80*F80</f>
-        <v>728</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D81" s="0" t="s">
@@ -2395,11 +2077,6 @@
       </c>
       <c r="E81" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F81" s="4"/>
-      <c r="G81" s="1" t="n">
-        <f aca="false">E81*F81</f>
-        <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,23 +2086,19 @@
       <c r="E82" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F82" s="4" t="n">
+      <c r="F82" s="0" t="n">
         <f aca="false">A82</f>
         <v>283</v>
       </c>
-      <c r="G82" s="1" t="n">
-        <f aca="false">E82*F82</f>
-        <v>283</v>
-      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D83" s="0" t="s">
@@ -2433,11 +2106,6 @@
       </c>
       <c r="E83" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F83" s="4"/>
-      <c r="G83" s="1" t="n">
-        <f aca="false">E83*F83</f>
-        <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2447,23 +2115,19 @@
       <c r="E84" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F84" s="4" t="n">
+      <c r="F84" s="0" t="n">
         <f aca="false">A84</f>
         <v>1267</v>
       </c>
-      <c r="G84" s="1" t="n">
-        <f aca="false">E84*F84</f>
-        <v>1267</v>
-      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D85" s="0" t="s">
@@ -2471,11 +2135,6 @@
       </c>
       <c r="E85" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F85" s="4"/>
-      <c r="G85" s="1" t="n">
-        <f aca="false">E85*F85</f>
-        <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,23 +2144,19 @@
       <c r="E86" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F86" s="4" t="n">
+      <c r="F86" s="0" t="n">
         <f aca="false">A86</f>
         <v>335</v>
       </c>
-      <c r="G86" s="1" t="n">
-        <f aca="false">E86*F86</f>
-        <v>335</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D87" s="0" t="s">
@@ -2509,11 +2164,6 @@
       </c>
       <c r="E87" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F87" s="4"/>
-      <c r="G87" s="1" t="n">
-        <f aca="false">E87*F87</f>
-        <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,23 +2173,19 @@
       <c r="E88" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F88" s="4" t="n">
+      <c r="F88" s="0" t="n">
         <f aca="false">A88</f>
         <v>1395</v>
       </c>
-      <c r="G88" s="1" t="n">
-        <f aca="false">E88*F88</f>
-        <v>1395</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D89" s="0" t="s">
@@ -2547,11 +2193,6 @@
       </c>
       <c r="E89" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F89" s="4"/>
-      <c r="G89" s="1" t="n">
-        <f aca="false">E89*F89</f>
-        <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,23 +2202,19 @@
       <c r="E90" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F90" s="4" t="n">
+      <c r="F90" s="0" t="n">
         <f aca="false">A90</f>
         <v>133</v>
       </c>
-      <c r="G90" s="1" t="n">
-        <f aca="false">E90*F90</f>
-        <v>133</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D91" s="0" t="s">
@@ -2585,14 +2222,6 @@
       </c>
       <c r="E91" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F91" s="4"/>
-      <c r="G91" s="1" t="n">
-        <f aca="false">E91*F91</f>
-        <v>0</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,41 +2231,26 @@
       <c r="E92" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F92" s="4" t="n">
+      <c r="F92" s="0" t="n">
         <f aca="false">A92</f>
         <v>135</v>
       </c>
-      <c r="G92" s="1" t="n">
-        <f aca="false">E92*F92</f>
-        <v>135</v>
-      </c>
-      <c r="I92" s="2" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" s="0" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+      <c r="C93" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="D93" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="E93" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F93" s="4"/>
-      <c r="G93" s="1" t="n">
-        <f aca="false">E93*F93</f>
-        <v>0</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2646,35 +2260,26 @@
       <c r="E94" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F94" s="4" t="n">
+      <c r="F94" s="0" t="n">
         <f aca="false">A94</f>
         <v>542</v>
       </c>
-      <c r="G94" s="1" t="n">
-        <f aca="false">E94*F94</f>
-        <v>542</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="E95" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F95" s="4"/>
-      <c r="G95" s="1" t="n">
-        <f aca="false">E95*F95</f>
-        <v>0</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,35 +2289,26 @@
       <c r="E96" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F96" s="4" t="n">
+      <c r="F96" s="0" t="n">
         <f aca="false">A96</f>
         <v>714</v>
       </c>
-      <c r="G96" s="1" t="n">
-        <f aca="false">E96*F96</f>
-        <v>714</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D97" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>174</v>
-      </c>
       <c r="E97" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F97" s="4"/>
-      <c r="G97" s="1" t="n">
-        <f aca="false">E97*F97</f>
-        <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,35 +2318,26 @@
       <c r="E98" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F98" s="4" t="n">
+      <c r="F98" s="0" t="n">
         <f aca="false">A98</f>
         <v>352</v>
       </c>
-      <c r="G98" s="1" t="n">
-        <f aca="false">E98*F98</f>
-        <v>352</v>
-      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D99" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="E99" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F99" s="4"/>
-      <c r="G99" s="1" t="n">
-        <f aca="false">E99*F99</f>
-        <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2760,35 +2347,26 @@
       <c r="E100" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F100" s="4" t="n">
+      <c r="F100" s="0" t="n">
         <f aca="false">A100</f>
         <v>194</v>
       </c>
-      <c r="G100" s="1" t="n">
-        <f aca="false">E100*F100</f>
-        <v>194</v>
-      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D101" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B101" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>182</v>
-      </c>
       <c r="E101" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F101" s="4"/>
-      <c r="G101" s="1" t="n">
-        <f aca="false">E101*F101</f>
-        <v>0</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,35 +2376,26 @@
       <c r="E102" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F102" s="4" t="n">
+      <c r="F102" s="0" t="n">
         <f aca="false">A102</f>
         <v>216</v>
       </c>
-      <c r="G102" s="1" t="n">
-        <f aca="false">E102*F102</f>
-        <v>216</v>
-      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D103" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B103" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>186</v>
-      </c>
       <c r="E103" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F103" s="4"/>
-      <c r="G103" s="1" t="n">
-        <f aca="false">E103*F103</f>
-        <v>0</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,35 +2405,26 @@
       <c r="E104" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F104" s="4" t="n">
+      <c r="F104" s="0" t="n">
         <f aca="false">A104</f>
         <v>316</v>
       </c>
-      <c r="G104" s="1" t="n">
-        <f aca="false">E104*F104</f>
-        <v>316</v>
-      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D105" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B105" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>190</v>
-      </c>
       <c r="E105" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F105" s="4"/>
-      <c r="G105" s="1" t="n">
-        <f aca="false">E105*F105</f>
-        <v>0</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,35 +2434,26 @@
       <c r="E106" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F106" s="4" t="n">
+      <c r="F106" s="0" t="n">
         <f aca="false">A106</f>
         <v>366</v>
       </c>
-      <c r="G106" s="1" t="n">
-        <f aca="false">E106*F106</f>
-        <v>366</v>
-      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D107" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B107" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D107" s="0" t="s">
-        <v>194</v>
-      </c>
       <c r="E107" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F107" s="4"/>
-      <c r="G107" s="1" t="n">
-        <f aca="false">E107*F107</f>
-        <v>0</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,35 +2463,26 @@
       <c r="E108" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F108" s="4" t="n">
+      <c r="F108" s="0" t="n">
         <f aca="false">A108</f>
         <v>249</v>
       </c>
-      <c r="G108" s="1" t="n">
-        <f aca="false">E108*F108</f>
-        <v>249</v>
-      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B109" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>198</v>
-      </c>
       <c r="E109" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F109" s="4"/>
-      <c r="G109" s="1" t="n">
-        <f aca="false">E109*F109</f>
-        <v>0</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2950,35 +2492,26 @@
       <c r="E110" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F110" s="4" t="n">
+      <c r="F110" s="0" t="n">
         <f aca="false">A110</f>
         <v>141</v>
       </c>
-      <c r="G110" s="1" t="n">
-        <f aca="false">E110*F110</f>
-        <v>141</v>
-      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D111" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>202</v>
-      </c>
       <c r="E111" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F111" s="4"/>
-      <c r="G111" s="1" t="n">
-        <f aca="false">E111*F111</f>
-        <v>0</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,35 +2521,26 @@
       <c r="E112" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F112" s="4" t="n">
+      <c r="F112" s="0" t="n">
         <f aca="false">A112</f>
         <v>816</v>
       </c>
-      <c r="G112" s="1" t="n">
-        <f aca="false">E112*F112</f>
-        <v>816</v>
-      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D113" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>206</v>
-      </c>
       <c r="E113" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F113" s="4"/>
-      <c r="G113" s="1" t="n">
-        <f aca="false">E113*F113</f>
-        <v>0</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,35 +2550,26 @@
       <c r="E114" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F114" s="4" t="n">
+      <c r="F114" s="0" t="n">
         <f aca="false">A114</f>
         <v>253</v>
       </c>
-      <c r="G114" s="1" t="n">
-        <f aca="false">E114*F114</f>
-        <v>253</v>
-      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D115" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>210</v>
-      </c>
       <c r="E115" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F115" s="4"/>
-      <c r="G115" s="1" t="n">
-        <f aca="false">E115*F115</f>
-        <v>0</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,35 +2579,26 @@
       <c r="E116" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F116" s="4" t="n">
+      <c r="F116" s="0" t="n">
         <f aca="false">A116</f>
         <v>266</v>
       </c>
-      <c r="G116" s="1" t="n">
-        <f aca="false">E116*F116</f>
-        <v>266</v>
-      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D117" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B117" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>214</v>
-      </c>
       <c r="E117" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F117" s="4"/>
-      <c r="G117" s="1" t="n">
-        <f aca="false">E117*F117</f>
-        <v>0</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3102,35 +2608,26 @@
       <c r="E118" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F118" s="4" t="n">
+      <c r="F118" s="0" t="n">
         <f aca="false">A118</f>
         <v>686</v>
       </c>
-      <c r="G118" s="1" t="n">
-        <f aca="false">E118*F118</f>
-        <v>686</v>
-      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D119" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B119" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>218</v>
-      </c>
       <c r="E119" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F119" s="4"/>
-      <c r="G119" s="1" t="n">
-        <f aca="false">E119*F119</f>
-        <v>0</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,35 +2637,26 @@
       <c r="E120" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F120" s="4" t="n">
+      <c r="F120" s="0" t="n">
         <f aca="false">A120</f>
         <v>108</v>
       </c>
-      <c r="G120" s="1" t="n">
-        <f aca="false">E120*F120</f>
-        <v>108</v>
-      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D121" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B121" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D121" s="0" t="s">
-        <v>222</v>
-      </c>
       <c r="E121" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F121" s="4"/>
-      <c r="G121" s="1" t="n">
-        <f aca="false">E121*F121</f>
-        <v>0</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3178,35 +2666,26 @@
       <c r="E122" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F122" s="4" t="n">
+      <c r="F122" s="0" t="n">
         <f aca="false">A122</f>
         <v>590</v>
       </c>
-      <c r="G122" s="1" t="n">
-        <f aca="false">E122*F122</f>
-        <v>590</v>
-      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D123" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>226</v>
-      </c>
       <c r="E123" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F123" s="4"/>
-      <c r="G123" s="1" t="n">
-        <f aca="false">E123*F123</f>
-        <v>0</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,35 +2695,26 @@
       <c r="E124" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F124" s="4" t="n">
+      <c r="F124" s="0" t="n">
         <f aca="false">A124</f>
         <v>280</v>
       </c>
-      <c r="G124" s="1" t="n">
-        <f aca="false">E124*F124</f>
-        <v>280</v>
-      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D125" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B125" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D125" s="0" t="s">
-        <v>230</v>
-      </c>
       <c r="E125" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F125" s="4"/>
-      <c r="G125" s="1" t="n">
-        <f aca="false">E125*F125</f>
-        <v>0</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3254,35 +2724,26 @@
       <c r="E126" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F126" s="4" t="n">
+      <c r="F126" s="0" t="n">
         <f aca="false">A126</f>
         <v>225</v>
       </c>
-      <c r="G126" s="1" t="n">
-        <f aca="false">E126*F126</f>
-        <v>225</v>
-      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D127" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="B127" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>234</v>
-      </c>
       <c r="E127" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="F127" s="4"/>
-      <c r="G127" s="1" t="n">
-        <f aca="false">E127*F127</f>
-        <v>0</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3292,26 +2753,192 @@
       <c r="E128" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F128" s="4" t="n">
+      <c r="F128" s="0" t="n">
         <f aca="false">A128</f>
         <v>608</v>
       </c>
-      <c r="G128" s="1" t="n">
-        <f aca="false">E128*F128</f>
-        <v>608</v>
-      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G129" s="1" t="n">
-        <f aca="false">SUM(G1:G128)</f>
-        <v>38115</v>
+      <c r="A129" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>292</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <f aca="false">A130</f>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E131" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>1465</v>
+      </c>
+      <c r="E132" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <f aca="false">A132</f>
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>576</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <f aca="false">A134</f>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <f aca="false">A136</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E137" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <f aca="false">A138</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>506</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <f aca="false">A140</f>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F141" s="0" t="n">
+        <f aca="false">SUM(F1:F140)</f>
+        <v>41391</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I91" r:id="rId1" display="https://www.wildberries.ru/catalog/137790056/detail.aspx?size=234503434"/>
-    <hyperlink ref="I92" r:id="rId2" display="https://www.wildberries.ru/catalog/122932874/detail.aspx?size=216462701"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>